<commit_message>
Added drawings dimensions, changed footprint of op amp, and cleaned up
</commit_message>
<xml_diff>
--- a/Board/PowerSenseModule/bom/Inventory.xlsx
+++ b/Board/PowerSenseModule/bom/Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\Git\HKN-SAE-Project\Board\PowerSenseModule\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\904pa\Documents\Git\HKN-SAE-Project\Board\PowerSenseModule\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C342B356-B20E-4ADB-A96C-6CB61D2BC9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14C707C-12B4-44BC-B6E3-F532C4B0845B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -786,23 +786,23 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" customWidth="1"/>
-    <col min="4" max="4" width="72.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -822,7 +822,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -842,7 +842,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -862,7 +862,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -882,7 +882,7 @@
         <v>885012206092</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -902,7 +902,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -922,7 +922,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>8</v>
       </c>
@@ -942,7 +942,7 @@
         <v>885012206081</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>92</v>
       </c>
@@ -962,7 +962,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -982,7 +982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>13</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>110</v>
@@ -1220,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>13</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>13</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>16</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>13</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>8</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>14</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>14</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>3</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>5110</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>6</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>5</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3</v>
       </c>

</xml_diff>